<commit_message>
added export-function for networks to gephi
</commit_message>
<xml_diff>
--- a/Notizen/Vokabeln.xlsx
+++ b/Notizen/Vokabeln.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Leverage</t>
   </si>
@@ -296,6 +299,36 @@
   </si>
   <si>
     <t>unverpfändet</t>
+  </si>
+  <si>
+    <t>delinquencies</t>
+  </si>
+  <si>
+    <t>Nichtzahlung bei Fälligkeit</t>
+  </si>
+  <si>
+    <t>interest rate</t>
+  </si>
+  <si>
+    <t>Zinssatz</t>
+  </si>
+  <si>
+    <t>ameliorate</t>
+  </si>
+  <si>
+    <t>ausbessern</t>
+  </si>
+  <si>
+    <t>bailout</t>
+  </si>
+  <si>
+    <t>Notverkauf</t>
+  </si>
+  <si>
+    <t>equity</t>
+  </si>
+  <si>
+    <t>Eigenanteil</t>
   </si>
 </sst>
 </file>
@@ -335,10 +368,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -637,395 +698,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>74</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>60</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>62</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>68</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>82</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>0</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>84</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>75</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>90</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B36" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>24</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>80</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B40" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>78</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B43" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>20</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>42</v>
-      </c>
-      <c r="B40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>88</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B51" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>66</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B52" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>58</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B53" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>